<commit_message>
Revert "recommit Fixbug #130286" excel output
This reverts commit f5c38780b737e4800345eb9e687d38462d7e2946.
</commit_message>
<xml_diff>
--- a/nts.uk/uk.com/com.file/nts.uk.file.com.infra/out/production/resources/report/申請者として承認ルートのEXCEL出力.xlsx
+++ b/nts.uk/uk.com/com.file/nts.uk.file.com.infra/out/production/resources/report/申請者として承認ルートのEXCEL出力.xlsx
@@ -376,14 +376,14 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="ＭＳ Ｐゴシック"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="ＭＳ Ｐゴシック"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -391,7 +391,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="ＭＳ Ｐゴシック"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -399,7 +399,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="ＭＳ Ｐゴシック"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -412,7 +412,7 @@
     </font>
     <font>
       <sz val="6"/>
-      <name val="Calibri"/>
+      <name val="ＭＳ Ｐゴシック"/>
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -440,7 +440,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="ＭＳ Ｐゴシック"/>
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -677,11 +677,9 @@
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ"/>
-      <sheetName val="master"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0"/>
-      <sheetData sheetId="1" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -44539,28 +44537,28 @@
   <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" view="pageLayout" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="R7" sqref="R7"/>
+      <selection activeCell="T3" sqref="S3:T3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.7109375" defaultRowHeight="12"/>
+  <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="12"/>
   <cols>
-    <col min="1" max="1" width="1.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="1.625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.125" style="1" customWidth="1"/>
     <col min="4" max="4" width="11" style="1" customWidth="1"/>
-    <col min="5" max="5" width="6.85546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="6.85546875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="14.5703125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="6.85546875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="14.5703125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="6.85546875" style="1" customWidth="1"/>
-    <col min="12" max="12" width="14.5703125" style="1" customWidth="1"/>
-    <col min="13" max="13" width="6.85546875" style="1" customWidth="1"/>
-    <col min="14" max="14" width="14.5703125" style="1" customWidth="1"/>
-    <col min="15" max="15" width="14.42578125" style="1" customWidth="1"/>
-    <col min="16" max="16" width="1.5703125" style="1" customWidth="1"/>
-    <col min="17" max="16384" width="2.7109375" style="1"/>
+    <col min="5" max="5" width="6.875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14.625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="6.875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="14.625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="6.875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="14.625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="6.875" style="1" customWidth="1"/>
+    <col min="12" max="12" width="14.625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="6.875" style="1" customWidth="1"/>
+    <col min="14" max="14" width="14.625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="8.375" style="1" customWidth="1"/>
+    <col min="16" max="16" width="1.625" style="1" customWidth="1"/>
+    <col min="17" max="16384" width="2.75" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="15" customHeight="1" thickBot="1">
@@ -44621,7 +44619,7 @@
   <pageMargins left="0.39370078740157499" right="0.39370078740157499" top="0.59055118110236204" bottom="0.59055118110236204" header="0.31496062992126" footer="0.31496062992126"/>
   <pageSetup paperSize="9" scale="83" orientation="landscape" r:id="rId1"/>
   <headerFooter>
-    <oddHeader>&amp;C&amp;"ＭＳ ゴシック,太字"&amp;16承認者一覧（申請者）&amp;R&amp;"ＭＳ ゴシック,標準"&amp;9&amp;D &amp;T
+    <oddHeader>&amp;C&amp;"ＭＳ ゴシック,太字"&amp;16承認者一覧（申請者&amp;"-,標準"&amp;11）&amp;R&amp;"ＭＳ ゴシック,標準"&amp;9&amp;D &amp;T
 &amp;P/&amp;N</oddHeader>
   </headerFooter>
 </worksheet>

</xml_diff>